<commit_message>
fix: :art: update script
</commit_message>
<xml_diff>
--- a/resultados_comparacao_docentes.xlsx
+++ b/resultados_comparacao_docentes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,9 +433,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="32" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="120" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="70" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="38" customWidth="1" min="9" max="9"/>
+    <col width="24" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,43 +458,380 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Arquivos</t>
+          <t>Nícolas Oliveira de Araújo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ítalo Moraes Rocha Guedes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Toshik Iarley da Silva</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Genaina Aparecida de Souza</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Josimar Aleixo da Silva</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ariana Mota Pereira</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Marilia Cecilia de Souza Bittencourt</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Vinícius Martins Silva</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Catarine Markus</t>
+          <t>Adriano Perin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ok</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nenhum</t>
+          <t>1 citação(ões)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>PERIN, A. (1)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Ana Maria Mapeli</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>André Samuel Strassburger</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Arthur Bernardes Cecílio Filho</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4 citação(ões)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>FILHO, A (1)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>FILHO, A (1)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>FILHO, A (1)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>FILHO, A (1)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Diego Ismael Rocha</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Diego Silva Batista</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3 citação(ões)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CANDIDATO - Toshik Iarley da Silva.pdf, CANDIDATO - Toshik Iarley da Silva.pdf, CANDIDATO - Toshik Iarley da Silva.pdf</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4 citação(ões)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BATISTA, D. S. (1) | BATISTA, DIEGO S (1) | BATISTA, DIEGO SILVA (1)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BATISTA, D. S. (1)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Fernando Cesar Sala</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Guilherme da Silva Pereira</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Jackson Mirellys Azevêdo Souza</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1 citação(ões)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SOUZA, J. M. A. (1)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kassio Ferreira Mendes</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Leilson Costa Grangeiro</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Luis Felipe Villani Purquerio</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rumy Goto</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Simone da Costa Mello</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1 citação(ões)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MELLO, S. C. (1)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Thiago de Oliveira Vargas</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Ok</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: :bug: terminal close after processing
</commit_message>
<xml_diff>
--- a/resultados_comparacao_docentes.xlsx
+++ b/resultados_comparacao_docentes.xlsx
@@ -435,14 +435,14 @@
   <cols>
     <col width="32" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
-    <col width="28" customWidth="1" min="3" max="3"/>
-    <col width="27" customWidth="1" min="4" max="4"/>
-    <col width="70" customWidth="1" min="5" max="5"/>
-    <col width="28" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
-    <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="38" customWidth="1" min="9" max="9"/>
-    <col width="24" customWidth="1" min="10" max="10"/>
+    <col width="70" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="27" customWidth="1" min="6" max="6"/>
+    <col width="38" customWidth="1" min="7" max="7"/>
+    <col width="28" customWidth="1" min="8" max="8"/>
+    <col width="28" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,42 +458,42 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Toshik Iarley da Silva</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Vinícius Martins Silva</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ariana Mota Pereira</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Ítalo Moraes Rocha Guedes</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Marilia Cecilia de Souza Bittencourt</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Genaina Aparecida de Souza</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Nícolas Oliveira de Araújo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Ítalo Moraes Rocha Guedes</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Toshik Iarley da Silva</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Genaina Aparecida de Souza</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Josimar Aleixo da Silva</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Ariana Mota Pereira</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Marilia Cecilia de Souza Bittencourt</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Vinícius Martins Silva</t>
         </is>
       </c>
     </row>
@@ -509,17 +509,17 @@
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PERIN, A. (1)</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>PERIN, A. (1)</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -572,30 +572,30 @@
           <t>4 citação(ões)</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
         <is>
           <t>FILHO, A (1)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>FILHO, A (1)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>FILHO, A (1)</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>FILHO, A (1)</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -628,20 +628,20 @@
           <t>4 citação(ões)</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BATISTA, D. S. (1) | BATISTA, DIEGO SILVA (1) | BATISTA, DIEGO S (1)</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>BATISTA, D. S. (1) | BATISTA, DIEGO S (1) | BATISTA, DIEGO SILVA (1)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
         <is>
           <t>BATISTA, D. S. (1)</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
     </row>
@@ -697,13 +697,13 @@
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
         <is>
           <t>SOUZA, J. M. A. (1)</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
@@ -801,13 +801,13 @@
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
         <is>
           <t>MELLO, S. C. (1)</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>

</xml_diff>